<commit_message>
Branch and Bound - Final
</commit_message>
<xml_diff>
--- a/Time_compare_b&b.xlsx
+++ b/Time_compare_b&b.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wwishahi\Desktop\University\Master\2020 - 2021 Freshman\Algoirthmic softwares\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9440E56-8596-4342-8D38-31BA9EB83DAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C313FC3-3FDC-44A3-87A6-7369ACA65BDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8704798F-9F6B-4A25-AA65-B8278D734CE7}"/>
   </bookViews>
@@ -1909,8 +1909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F4E8C54-DE89-47E8-8C91-7344DDEF8C52}">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>